<commit_message>
Update map to reflect additions
</commit_message>
<xml_diff>
--- a/Map/Map.xlsx
+++ b/Map/Map.xlsx
@@ -5,7 +5,7 @@
   <workbookPr date1904="1" defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alex\Documents\GitHub\CSCI1101-group_project\Map\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alex's Desktop\Documents\GitHub\CSCI1101-group_project\Map\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,14 +19,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="191">
   <si>
     <t>Map of NS Fjord VValkyrie</t>
   </si>
   <si>
-    <t>Key</t>
-  </si>
-  <si>
     <t>Nisk</t>
   </si>
   <si>
@@ -36,9 +33,6 @@
     <t>Lock</t>
   </si>
   <si>
-    <t>Tough Guy</t>
-  </si>
-  <si>
     <t>Lock Caeven</t>
   </si>
   <si>
@@ -547,13 +541,64 @@
   </si>
   <si>
     <t>14,10</t>
+  </si>
+  <si>
+    <t>Weapon 8</t>
+  </si>
+  <si>
+    <t>Weapon 2</t>
+  </si>
+  <si>
+    <t>Weapon 3</t>
+  </si>
+  <si>
+    <t>Weapon 4</t>
+  </si>
+  <si>
+    <t>Weapon 5</t>
+  </si>
+  <si>
+    <t>Weapon 6</t>
+  </si>
+  <si>
+    <t>Weapon 7</t>
+  </si>
+  <si>
+    <t>Key1</t>
+  </si>
+  <si>
+    <t>Key2</t>
+  </si>
+  <si>
+    <t>Key3</t>
+  </si>
+  <si>
+    <t>Key4</t>
+  </si>
+  <si>
+    <t>Key5</t>
+  </si>
+  <si>
+    <t>Key6</t>
+  </si>
+  <si>
+    <t>Key7</t>
+  </si>
+  <si>
+    <t>Potion</t>
+  </si>
+  <si>
+    <t>Tough Enemy</t>
+  </si>
+  <si>
+    <t>Enemy</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color indexed="8"/>
@@ -579,8 +624,14 @@
       <color indexed="8"/>
       <name val="Helvetica"/>
     </font>
+    <font>
+      <sz val="15"/>
+      <color indexed="8"/>
+      <name val="Courier New"/>
+      <family val="3"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -617,6 +668,24 @@
         <bgColor auto="1"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF9966FF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00FFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="10">
     <border>
@@ -767,7 +836,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -813,9 +882,6 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -831,12 +897,6 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -844,6 +904,21 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -851,6 +926,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -925,6 +1009,10 @@
       <rgbColor rgb="00333399"/>
       <rgbColor rgb="00333333"/>
     </indexedColors>
+    <mruColors>
+      <color rgb="FF00FFCC"/>
+      <color rgb="FF9966FF"/>
+    </mruColors>
   </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -1205,8 +1293,8 @@
   </sheetPr>
   <dimension ref="A1:IV17"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A10" zoomScale="40" zoomScaleNormal="40" zoomScaleSheetLayoutView="10" workbookViewId="0">
-      <selection activeCell="N3" sqref="N3:X17"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="40" zoomScaleNormal="40" zoomScaleSheetLayoutView="10" workbookViewId="0">
+      <selection activeCell="Z5" sqref="Z5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.19921875" defaultRowHeight="43.9" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1220,120 +1308,128 @@
   <sheetData>
     <row r="1" spans="2:24" ht="29.1" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="2" spans="2:24" ht="52.5" x14ac:dyDescent="0.7">
-      <c r="B2" s="26" t="s">
+      <c r="B2" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="27"/>
-      <c r="D2" s="27"/>
-      <c r="E2" s="27"/>
-      <c r="F2" s="27"/>
-      <c r="G2" s="27"/>
-      <c r="H2" s="27"/>
-      <c r="I2" s="27"/>
-      <c r="J2" s="27"/>
-      <c r="K2" s="27"/>
-      <c r="L2" s="27"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="29"/>
+      <c r="E2" s="29"/>
+      <c r="F2" s="29"/>
+      <c r="G2" s="29"/>
+      <c r="H2" s="29"/>
+      <c r="I2" s="29"/>
+      <c r="J2" s="29"/>
+      <c r="K2" s="29"/>
+      <c r="L2" s="29"/>
     </row>
     <row r="3" spans="2:24" ht="99.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B3" s="2" t="s">
-        <v>1</v>
+        <v>181</v>
       </c>
       <c r="C3" s="3"/>
       <c r="D3" s="4" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E3" s="4"/>
       <c r="F3" s="3"/>
       <c r="G3" s="5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H3" s="3"/>
       <c r="I3" s="4"/>
-      <c r="J3" s="4"/>
+      <c r="J3" s="23" t="s">
+        <v>174</v>
+      </c>
       <c r="K3" s="3"/>
       <c r="L3" s="6" t="s">
-        <v>1</v>
+        <v>182</v>
       </c>
       <c r="N3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="O3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="P3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="O3" s="1" t="s">
+      <c r="Q3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="P3" s="1" t="s">
+      <c r="R3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="Q3" s="1" t="s">
+      <c r="S3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="R3" s="1" t="s">
+      <c r="T3" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="S3" s="1" t="s">
+      <c r="U3" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="T3" s="1" t="s">
+      <c r="V3" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="U3" s="1" t="s">
+      <c r="W3" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="V3" s="1" t="s">
+      <c r="X3" s="1" t="s">
         <v>19</v>
-      </c>
-      <c r="W3" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="X3" s="1" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="4" spans="2:24" ht="100.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B4" s="7"/>
-      <c r="C4" s="8"/>
+      <c r="C4" s="30" t="s">
+        <v>188</v>
+      </c>
       <c r="D4" s="8"/>
-      <c r="E4" s="8"/>
+      <c r="E4" s="32" t="s">
+        <v>190</v>
+      </c>
       <c r="F4" s="8"/>
       <c r="G4" s="9" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H4" s="8"/>
       <c r="I4" s="8"/>
       <c r="J4" s="8"/>
-      <c r="K4" s="8"/>
+      <c r="K4" s="30" t="s">
+        <v>188</v>
+      </c>
       <c r="L4" s="10"/>
       <c r="N4" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="O4" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="P4" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q4" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="P4" s="1" t="s">
+      <c r="R4" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="Q4" s="1" t="s">
+      <c r="S4" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="R4" s="1" t="s">
+      <c r="T4" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="S4" s="1" t="s">
+      <c r="U4" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="T4" s="1" t="s">
+      <c r="V4" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="U4" s="1" t="s">
+      <c r="W4" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="V4" s="1" t="s">
+      <c r="X4" s="1" t="s">
         <v>43</v>
-      </c>
-      <c r="W4" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="X4" s="1" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="5" spans="2:24" ht="100.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -1344,388 +1440,422 @@
       <c r="F5" s="12"/>
       <c r="G5" s="12"/>
       <c r="H5" s="12"/>
-      <c r="I5" s="8"/>
+      <c r="I5" s="32" t="s">
+        <v>190</v>
+      </c>
       <c r="J5" s="12"/>
       <c r="K5" s="12"/>
       <c r="L5" s="13"/>
       <c r="N5" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="O5" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="P5" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q5" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="P5" s="1" t="s">
+      <c r="R5" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="Q5" s="1" t="s">
+      <c r="S5" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="R5" s="1" t="s">
+      <c r="T5" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="S5" s="1" t="s">
+      <c r="U5" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="T5" s="1" t="s">
+      <c r="V5" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="U5" s="1" t="s">
+      <c r="W5" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="V5" s="1" t="s">
+      <c r="X5" s="1" t="s">
         <v>53</v>
-      </c>
-      <c r="W5" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="X5" s="1" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="6" spans="2:24" ht="100.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="7"/>
+      <c r="B6" s="32" t="s">
+        <v>190</v>
+      </c>
       <c r="C6" s="14" t="s">
-        <v>1</v>
+        <v>183</v>
       </c>
       <c r="D6" s="12"/>
       <c r="E6" s="8"/>
-      <c r="F6" s="15" t="s">
-        <v>5</v>
+      <c r="F6" s="31" t="s">
+        <v>189</v>
       </c>
       <c r="G6" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="H6" s="15" t="s">
-        <v>5</v>
+        <v>3</v>
+      </c>
+      <c r="H6" s="31" t="s">
+        <v>189</v>
       </c>
       <c r="I6" s="8"/>
       <c r="J6" s="12"/>
       <c r="K6" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="L6" s="10"/>
+        <v>4</v>
+      </c>
+      <c r="L6" s="32" t="s">
+        <v>190</v>
+      </c>
       <c r="N6" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="O6" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="P6" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q6" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="P6" s="1" t="s">
+      <c r="R6" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="Q6" s="1" t="s">
+      <c r="S6" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="R6" s="1" t="s">
+      <c r="T6" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="S6" s="1" t="s">
+      <c r="U6" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="T6" s="1" t="s">
+      <c r="V6" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="U6" s="1" t="s">
+      <c r="W6" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="V6" s="1" t="s">
+      <c r="X6" s="1" t="s">
         <v>63</v>
-      </c>
-      <c r="W6" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="X6" s="1" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="7" spans="2:24" ht="100.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B7" s="7"/>
       <c r="C7" s="12"/>
-      <c r="D7" s="8"/>
+      <c r="D7" s="27" t="s">
+        <v>178</v>
+      </c>
       <c r="E7" s="12"/>
       <c r="F7" s="12"/>
-      <c r="G7" s="16"/>
+      <c r="G7" s="15"/>
       <c r="H7" s="12"/>
       <c r="I7" s="12"/>
       <c r="J7" s="14" t="s">
-        <v>1</v>
+        <v>184</v>
       </c>
       <c r="K7" s="12"/>
       <c r="L7" s="10"/>
       <c r="N7" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="O7" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="P7" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="Q7" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="P7" s="1" t="s">
+      <c r="R7" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="Q7" s="1" t="s">
+      <c r="S7" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="R7" s="1" t="s">
+      <c r="T7" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="S7" s="1" t="s">
+      <c r="U7" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="T7" s="1" t="s">
+      <c r="V7" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="U7" s="1" t="s">
+      <c r="W7" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="V7" s="1" t="s">
+      <c r="X7" s="1" t="s">
         <v>73</v>
-      </c>
-      <c r="W7" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="X7" s="1" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="8" spans="2:24" ht="100.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B8" s="7"/>
+      <c r="B8" s="32" t="s">
+        <v>190</v>
+      </c>
       <c r="C8" s="8"/>
-      <c r="D8" s="8"/>
+      <c r="D8" s="32" t="s">
+        <v>190</v>
+      </c>
       <c r="E8" s="8"/>
       <c r="F8" s="8"/>
-      <c r="G8" s="8"/>
+      <c r="G8" s="32" t="s">
+        <v>190</v>
+      </c>
       <c r="H8" s="12"/>
-      <c r="I8" s="8"/>
+      <c r="I8" s="32" t="s">
+        <v>190</v>
+      </c>
       <c r="J8" s="8"/>
       <c r="K8" s="8"/>
-      <c r="L8" s="10"/>
+      <c r="L8" s="30" t="s">
+        <v>188</v>
+      </c>
       <c r="N8" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="O8" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="P8" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="Q8" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="P8" s="1" t="s">
+      <c r="R8" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="Q8" s="1" t="s">
+      <c r="S8" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="R8" s="1" t="s">
+      <c r="T8" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="S8" s="1" t="s">
+      <c r="U8" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="T8" s="1" t="s">
+      <c r="V8" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="U8" s="1" t="s">
+      <c r="W8" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="V8" s="1" t="s">
+      <c r="X8" s="1" t="s">
         <v>83</v>
-      </c>
-      <c r="W8" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="X8" s="1" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="9" spans="2:24" ht="100.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B9" s="11"/>
       <c r="C9" s="12"/>
-      <c r="D9" s="15" t="s">
-        <v>5</v>
+      <c r="D9" s="31" t="s">
+        <v>189</v>
       </c>
       <c r="E9" s="12"/>
       <c r="F9" s="12"/>
-      <c r="G9" s="8"/>
+      <c r="G9" s="30" t="s">
+        <v>188</v>
+      </c>
       <c r="H9" s="8"/>
       <c r="I9" s="8"/>
       <c r="J9" s="12"/>
       <c r="K9" s="12"/>
       <c r="L9" s="13"/>
       <c r="N9" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="O9" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="P9" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="Q9" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="P9" s="1" t="s">
+      <c r="R9" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="Q9" s="1" t="s">
+      <c r="S9" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="R9" s="1" t="s">
+      <c r="T9" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="S9" s="1" t="s">
+      <c r="U9" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="T9" s="1" t="s">
+      <c r="V9" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="U9" s="1" t="s">
+      <c r="W9" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="V9" s="1" t="s">
+      <c r="X9" s="1" t="s">
         <v>93</v>
-      </c>
-      <c r="W9" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="X9" s="1" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="10" spans="2:24" ht="100.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B10" s="17" t="s">
-        <v>1</v>
+      <c r="B10" s="16" t="s">
+        <v>185</v>
       </c>
       <c r="C10" s="12"/>
       <c r="D10" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="E10" s="16"/>
+        <v>3</v>
+      </c>
+      <c r="E10" s="15"/>
       <c r="F10" s="12"/>
       <c r="G10" s="12"/>
       <c r="H10" s="12"/>
       <c r="I10" s="8" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="J10" s="12"/>
-      <c r="K10" s="8"/>
+      <c r="K10" s="32" t="s">
+        <v>190</v>
+      </c>
       <c r="L10" s="13"/>
       <c r="N10" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="O10" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="P10" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="Q10" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="P10" s="1" t="s">
+      <c r="R10" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="Q10" s="1" t="s">
+      <c r="S10" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="R10" s="1" t="s">
+      <c r="T10" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="S10" s="1" t="s">
+      <c r="U10" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="T10" s="1" t="s">
+      <c r="V10" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="U10" s="1" t="s">
+      <c r="W10" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="V10" s="1" t="s">
+      <c r="X10" s="1" t="s">
         <v>103</v>
-      </c>
-      <c r="W10" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="X10" s="1" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="11" spans="2:24" ht="100.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B11" s="18"/>
+      <c r="B11" s="17"/>
       <c r="C11" s="12"/>
       <c r="D11" s="12"/>
       <c r="E11" s="8"/>
-      <c r="F11" s="8"/>
+      <c r="F11" s="27" t="s">
+        <v>179</v>
+      </c>
       <c r="G11" s="8"/>
       <c r="H11" s="8" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="I11" s="12"/>
       <c r="J11" s="14" t="s">
-        <v>1</v>
+        <v>186</v>
       </c>
       <c r="K11" s="8"/>
-      <c r="L11" s="10"/>
+      <c r="L11" s="25" t="s">
+        <v>176</v>
+      </c>
       <c r="N11" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="O11" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="P11" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="Q11" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="P11" s="1" t="s">
+      <c r="R11" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="Q11" s="1" t="s">
+      <c r="S11" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="R11" s="1" t="s">
+      <c r="T11" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="S11" s="1" t="s">
+      <c r="U11" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="T11" s="1" t="s">
+      <c r="V11" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="U11" s="1" t="s">
+      <c r="W11" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="V11" s="1" t="s">
+      <c r="X11" s="1" t="s">
         <v>113</v>
-      </c>
-      <c r="W11" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="X11" s="1" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="12" spans="2:24" ht="99.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B12" s="7"/>
-      <c r="C12" s="8"/>
-      <c r="D12" s="8"/>
-      <c r="E12" s="8"/>
+      <c r="C12" s="32" t="s">
+        <v>190</v>
+      </c>
+      <c r="D12" s="30" t="s">
+        <v>188</v>
+      </c>
+      <c r="E12" s="32" t="s">
+        <v>190</v>
+      </c>
       <c r="F12" s="12"/>
       <c r="G12" s="12"/>
       <c r="H12" s="12"/>
       <c r="I12" s="12"/>
       <c r="J12" s="12"/>
-      <c r="K12" s="8"/>
+      <c r="K12" s="32" t="s">
+        <v>190</v>
+      </c>
       <c r="L12" s="13"/>
       <c r="N12" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="O12" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="P12" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="Q12" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="P12" s="1" t="s">
+      <c r="R12" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="Q12" s="1" t="s">
+      <c r="S12" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="R12" s="1" t="s">
+      <c r="T12" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="S12" s="1" t="s">
+      <c r="U12" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="T12" s="1" t="s">
+      <c r="V12" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="U12" s="1" t="s">
+      <c r="W12" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="V12" s="1" t="s">
+      <c r="X12" s="1" t="s">
         <v>123</v>
-      </c>
-      <c r="W12" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="X12" s="1" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="13" spans="2:24" ht="99.4" customHeight="1" x14ac:dyDescent="0.2">
@@ -1735,95 +1865,105 @@
       <c r="E13" s="8"/>
       <c r="F13" s="12"/>
       <c r="G13" s="8"/>
-      <c r="H13" s="8"/>
-      <c r="I13" s="8"/>
+      <c r="H13" s="30" t="s">
+        <v>188</v>
+      </c>
+      <c r="I13" s="32" t="s">
+        <v>190</v>
+      </c>
       <c r="J13" s="12"/>
       <c r="K13" s="8"/>
       <c r="L13" s="13"/>
       <c r="N13" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="O13" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="P13" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="Q13" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="P13" s="1" t="s">
+      <c r="R13" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="Q13" s="1" t="s">
+      <c r="S13" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="R13" s="1" t="s">
+      <c r="T13" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="S13" s="1" t="s">
+      <c r="U13" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="T13" s="1" t="s">
+      <c r="V13" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="U13" s="1" t="s">
+      <c r="W13" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="V13" s="1" t="s">
+      <c r="X13" s="1" t="s">
         <v>133</v>
-      </c>
-      <c r="W13" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="X13" s="1" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="14" spans="2:24" ht="99.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B14" s="11"/>
-      <c r="C14" s="16"/>
+      <c r="C14" s="32" t="s">
+        <v>190</v>
+      </c>
       <c r="D14" s="8"/>
-      <c r="E14" s="8"/>
+      <c r="E14" s="27" t="s">
+        <v>180</v>
+      </c>
       <c r="F14" s="12"/>
-      <c r="G14" s="8"/>
+      <c r="G14" s="32" t="s">
+        <v>190</v>
+      </c>
       <c r="H14" s="12"/>
-      <c r="I14" s="19" t="s">
-        <v>9</v>
+      <c r="I14" s="18" t="s">
+        <v>7</v>
       </c>
       <c r="J14" s="12"/>
       <c r="K14" s="14" t="s">
-        <v>1</v>
-      </c>
-      <c r="L14" s="20" t="s">
-        <v>10</v>
+        <v>187</v>
+      </c>
+      <c r="L14" s="19" t="s">
+        <v>8</v>
       </c>
       <c r="N14" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="O14" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="P14" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="Q14" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="P14" s="1" t="s">
+      <c r="R14" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="Q14" s="1" t="s">
+      <c r="S14" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="R14" s="1" t="s">
+      <c r="T14" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="S14" s="1" t="s">
+      <c r="U14" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="T14" s="1" t="s">
+      <c r="V14" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="U14" s="1" t="s">
+      <c r="W14" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="V14" s="1" t="s">
+      <c r="X14" s="1" t="s">
         <v>143</v>
-      </c>
-      <c r="W14" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="X14" s="1" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="15" spans="2:24" ht="99.4" customHeight="1" x14ac:dyDescent="0.2">
@@ -1832,140 +1972,158 @@
       <c r="D15" s="12"/>
       <c r="E15" s="12"/>
       <c r="F15" s="12"/>
-      <c r="G15" s="8"/>
+      <c r="G15" s="32" t="s">
+        <v>190</v>
+      </c>
       <c r="H15" s="12"/>
       <c r="I15" s="12"/>
-      <c r="J15" s="8"/>
+      <c r="J15" s="30" t="s">
+        <v>188</v>
+      </c>
       <c r="K15" s="8"/>
       <c r="L15" s="13"/>
       <c r="N15" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="O15" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="P15" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="Q15" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="P15" s="1" t="s">
+      <c r="R15" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="Q15" s="1" t="s">
+      <c r="S15" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="R15" s="1" t="s">
+      <c r="T15" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="S15" s="1" t="s">
+      <c r="U15" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="T15" s="1" t="s">
+      <c r="V15" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="U15" s="1" t="s">
+      <c r="W15" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="V15" s="1" t="s">
+      <c r="X15" s="1" t="s">
         <v>153</v>
-      </c>
-      <c r="W15" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="X15" s="1" t="s">
-        <v>155</v>
       </c>
     </row>
     <row r="16" spans="2:24" ht="99.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B16" s="11"/>
-      <c r="C16" s="16"/>
+      <c r="C16" s="32" t="s">
+        <v>190</v>
+      </c>
       <c r="D16" s="12"/>
-      <c r="E16" s="15" t="s">
-        <v>5</v>
+      <c r="E16" s="31" t="s">
+        <v>189</v>
       </c>
       <c r="F16" s="9" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G16" s="8"/>
-      <c r="H16" s="8"/>
+      <c r="H16" s="32" t="s">
+        <v>190</v>
+      </c>
       <c r="I16" s="8"/>
-      <c r="J16" s="8"/>
+      <c r="J16" s="32" t="s">
+        <v>190</v>
+      </c>
       <c r="K16" s="8"/>
-      <c r="L16" s="21"/>
+      <c r="L16" s="32" t="s">
+        <v>190</v>
+      </c>
       <c r="N16" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="O16" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="P16" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="Q16" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="P16" s="1" t="s">
+      <c r="R16" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="Q16" s="1" t="s">
+      <c r="S16" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="R16" s="1" t="s">
+      <c r="T16" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="S16" s="1" t="s">
+      <c r="U16" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="T16" s="1" t="s">
+      <c r="V16" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="U16" s="1" t="s">
+      <c r="W16" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="V16" s="1" t="s">
+      <c r="X16" s="1" t="s">
         <v>163</v>
-      </c>
-      <c r="W16" s="1" t="s">
-        <v>164</v>
-      </c>
-      <c r="X16" s="1" t="s">
-        <v>165</v>
       </c>
     </row>
     <row r="17" spans="2:24" ht="99.4" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B17" s="22"/>
-      <c r="C17" s="23"/>
-      <c r="D17" s="23"/>
-      <c r="E17" s="23"/>
-      <c r="F17" s="24"/>
-      <c r="G17" s="23"/>
-      <c r="H17" s="24"/>
-      <c r="I17" s="23"/>
-      <c r="J17" s="24"/>
-      <c r="K17" s="24"/>
-      <c r="L17" s="25"/>
+      <c r="B17" s="26" t="s">
+        <v>177</v>
+      </c>
+      <c r="C17" s="20"/>
+      <c r="D17" s="32" t="s">
+        <v>190</v>
+      </c>
+      <c r="E17" s="20"/>
+      <c r="F17" s="21"/>
+      <c r="G17" s="20"/>
+      <c r="H17" s="21"/>
+      <c r="I17" s="24" t="s">
+        <v>175</v>
+      </c>
+      <c r="J17" s="21"/>
+      <c r="K17" s="21"/>
+      <c r="L17" s="22"/>
       <c r="N17" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="O17" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="P17" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="Q17" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="P17" s="1" t="s">
+      <c r="R17" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="Q17" s="1" t="s">
+      <c r="S17" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="R17" s="1" t="s">
+      <c r="T17" s="1" t="s">
         <v>169</v>
       </c>
-      <c r="S17" s="1" t="s">
+      <c r="U17" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="T17" s="1" t="s">
+      <c r="V17" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="U17" s="1" t="s">
+      <c r="W17" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="V17" s="1" t="s">
+      <c r="X17" s="1" t="s">
         <v>173</v>
-      </c>
-      <c r="W17" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="X17" s="1" t="s">
-        <v>175</v>
       </c>
     </row>
   </sheetData>

</xml_diff>